<commit_message>
Sustituidos datos por los nuevos observacion de arturo
</commit_message>
<xml_diff>
--- a/datos/medidas.xlsx
+++ b/datos/medidas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\notebooks\personal\cursos\inter-asun\PROYECTO INTERFEROMETRIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\notebooks\Paper interferometria\Interferometria - GUA\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9306BBD4-032D-447A-AB9F-930900DF30D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9777E19-9AB4-4100-A8ED-C7D109315AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabla" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
   <si>
     <t>Imagen</t>
   </si>
@@ -49,70 +49,34 @@
     <t>Notas</t>
   </si>
   <si>
-    <t xml:space="preserve">Sirio </t>
-  </si>
-  <si>
     <t xml:space="preserve">Halfa-7 nm </t>
   </si>
   <si>
-    <t xml:space="preserve">I </t>
-  </si>
-  <si>
-    <t xml:space="preserve">H </t>
-  </si>
-  <si>
-    <t xml:space="preserve">G </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rigel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">E </t>
-  </si>
-  <si>
-    <t>Doble</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Halfa-35 nm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">F </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Betelgeuse </t>
-  </si>
-  <si>
-    <t xml:space="preserve">B/L+C </t>
-  </si>
-  <si>
     <t>4X</t>
   </si>
   <si>
-    <t xml:space="preserve">B </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hbeta-8.5nm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">D </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GammaLeo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sF </t>
-  </si>
-  <si>
-    <t xml:space="preserve">- </t>
-  </si>
-  <si>
-    <t>Estrella</t>
+    <t>Arturo</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>no simetrico</t>
+  </si>
+  <si>
+    <t>contiguos b</t>
+  </si>
+  <si>
+    <t>fuera de eje</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>a Borde no encaja</t>
   </si>
 </sst>
 </file>
@@ -495,8 +459,8 @@
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,106 +505,120 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F2" s="5">
-        <v>220</v>
+        <v>310</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="5">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F3" s="5">
-        <v>158</v>
+        <v>230</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="4"/>
+      <c r="I3" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
+      <c r="D4" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="5">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="F4" s="5">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>14</v>
+      <c r="B5" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E5" s="5">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="F5" s="5">
-        <v>222</v>
+        <v>270</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
+      <c r="B6" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5">
+        <v>30</v>
+      </c>
+      <c r="F6" s="6">
+        <v>190</v>
+      </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="2" t="s">
@@ -651,467 +629,270 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>18</v>
+      <c r="B7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E7" s="5">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="F7" s="5">
-        <v>147</v>
+        <v>60</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>15</v>
+      <c r="B8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E8" s="5">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="F8" s="5">
-        <v>222</v>
+        <v>40</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>18</v>
+      <c r="B9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E9" s="5">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="F9" s="5">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>20</v>
+      <c r="B10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E10" s="5">
         <v>30</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="5">
-        <v>133</v>
-      </c>
-      <c r="H10" s="5">
-        <v>238</v>
-      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="4" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="5">
-        <v>30</v>
-      </c>
-      <c r="F11" s="5">
-        <v>238</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="5">
-        <v>30</v>
-      </c>
-      <c r="F12" s="5">
-        <v>133</v>
-      </c>
+      <c r="A12" s="5"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="5">
-        <v>30</v>
-      </c>
-      <c r="F13" s="5">
-        <v>133</v>
-      </c>
+      <c r="A13" s="5"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="5">
-        <v>51</v>
-      </c>
-      <c r="F14" s="5">
-        <v>147</v>
-      </c>
+      <c r="A14" s="5"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="5">
-        <v>30</v>
-      </c>
-      <c r="F15" s="5">
-        <v>238</v>
-      </c>
+      <c r="A15" s="5"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="5">
-        <v>30</v>
-      </c>
-      <c r="F16" s="5">
-        <v>133</v>
-      </c>
+      <c r="A16" s="5"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="5">
-        <v>50</v>
-      </c>
-      <c r="F17" s="5">
-        <v>222</v>
-      </c>
+      <c r="A17" s="5"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="5">
-        <v>65</v>
-      </c>
-      <c r="F18" s="5">
-        <v>162</v>
-      </c>
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="5">
-        <v>30</v>
-      </c>
-      <c r="F19" s="5">
-        <v>133</v>
-      </c>
+      <c r="A19" s="5"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="5">
-        <v>66</v>
-      </c>
-      <c r="F20" s="5">
-        <v>162</v>
-      </c>
+      <c r="A20" s="5"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="5">
-        <v>66</v>
-      </c>
-      <c r="F21" s="5">
-        <v>162</v>
-      </c>
+      <c r="A21" s="5"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="5">
-        <v>66</v>
-      </c>
-      <c r="F22" s="5">
-        <v>205</v>
-      </c>
+      <c r="A22" s="5"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="5">
-        <v>90</v>
-      </c>
-      <c r="F23" s="5">
-        <v>187</v>
-      </c>
+      <c r="A23" s="5"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="5">
-        <v>90</v>
-      </c>
-      <c r="F24" s="5">
-        <v>187</v>
-      </c>
+      <c r="A24" s="5"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="5">
-        <v>51</v>
-      </c>
-      <c r="F25" s="5">
-        <v>147</v>
-      </c>
+      <c r="A25" s="5"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="A26" s="5"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
-      <c r="I26" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="I26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>